<commit_message>
Full suite of unittests run to confirm operation.
</commit_message>
<xml_diff>
--- a/hast2_1/tests/STAGES_v220/stage1_v220/HAST Inputs_stage1_v220.xlsx
+++ b/hast2_1/tests/STAGES_v220/stage1_v220/HAST Inputs_stage1_v220.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D43F4D6-80BA-41B4-BB46-04F4F52078B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA2F1C3-63C0-48CE-895F-7656820B2583}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -2439,8 +2439,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2591,6 +2591,9 @@
       <c r="D22" s="3"/>
     </row>
   </sheetData>
+  <sortState ref="A5:D7">
+    <sortCondition ref="A5:A7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -6243,8 +6246,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9583,17 +9586,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9602,7 +9594,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9754,23 +9746,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -9778,7 +9765,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9794,4 +9781,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>